<commit_message>
budget_26_v3.py final version of the 2026 budget. This version includes the following changes:
</commit_message>
<xml_diff>
--- a/Property Base rent SQFT.xlsx
+++ b/Property Base rent SQFT.xlsx
@@ -1,34 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/germanmontoya/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/germanmontoya/Python/vscode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A463D1-7E6A-4147-8068-69CCDAC00AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5136FAA-9224-C346-8563-1DABA6DA659F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16660" xr2:uid="{7FC1ED55-09A5-4909-89F9-1FB7800157C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1:$A$31</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$F$2:$F$31</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$F$2:$F$31</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$1:$A$31</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$F$2:$F$31</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$1:$A$31</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$F$2:$F$31</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$A$2:$A$31</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -50,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>ATS</t>
   </si>
@@ -158,16 +144,21 @@
   </si>
   <si>
     <t>Slope</t>
+  </si>
+  <si>
+    <t>avg_SQFT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +168,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -229,10 +227,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -246,9 +245,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -581,19 +589,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AEFD23-296D-41E5-93A7-66947C4E1891}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.83203125" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -609,638 +621,761 @@
       <c r="E1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="5">
         <v>337</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="5">
         <v>864</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="6">
         <v>1532</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="6">
         <v>1908</v>
       </c>
-      <c r="F2" s="5">
-        <f>(E2-D2)/(C2-B2)</f>
+      <c r="F2" s="7">
+        <f t="shared" ref="F2:F31" si="0">(E2-D2)/(C2-B2)</f>
         <v>0.71347248576850097</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="5">
+        <f>AVERAGE(B2:C2)</f>
+        <v>600.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="5">
         <v>527</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="5">
         <v>1486</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="6">
         <v>1035</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="6">
         <v>2030</v>
       </c>
-      <c r="F3" s="5">
-        <f>(E3-D3)/(C3-B3)</f>
+      <c r="F3" s="7">
+        <f t="shared" si="0"/>
         <v>1.0375391032325338</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="5">
+        <f t="shared" ref="G3:G31" si="1">AVERAGE(B3:C3)</f>
+        <v>1006.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="5">
         <v>703</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="5">
         <v>1321</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="6">
         <v>1403</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="6">
         <v>2100</v>
       </c>
-      <c r="F4" s="5">
-        <f>(E4-D4)/(C4-B4)</f>
+      <c r="F4" s="7">
+        <f t="shared" si="0"/>
         <v>1.1278317152103561</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="5">
+        <f t="shared" si="1"/>
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="5">
         <v>712</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="5">
         <v>1302</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="6">
         <v>1694</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="6">
         <v>2405</v>
       </c>
-      <c r="F5" s="5">
-        <f>(E5-D5)/(C5-B5)</f>
+      <c r="F5" s="7">
+        <f t="shared" si="0"/>
         <v>1.2050847457627119</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="5">
+        <f t="shared" si="1"/>
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="5">
         <v>755</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="5">
         <v>885</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="6">
         <v>1457</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="6">
         <v>1619</v>
       </c>
-      <c r="F6" s="5">
-        <f>(E6-D6)/(C6-B6)</f>
+      <c r="F6" s="7">
+        <f t="shared" si="0"/>
         <v>1.2461538461538462</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="5">
+        <f t="shared" si="1"/>
+        <v>820</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="5">
         <v>638</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="5">
         <v>1080</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="6">
         <v>1344</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="6">
         <v>1936</v>
       </c>
-      <c r="F7" s="5">
-        <f>(E7-D7)/(C7-B7)</f>
+      <c r="F7" s="7">
+        <f t="shared" si="0"/>
         <v>1.339366515837104</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="5">
+        <f t="shared" si="1"/>
+        <v>859</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="5">
         <v>830</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="5">
         <v>1236</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="6">
         <v>1619</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="6">
         <v>2167</v>
       </c>
-      <c r="F8" s="5">
-        <f>(E8-D8)/(C8-B8)</f>
+      <c r="F8" s="7">
+        <f t="shared" si="0"/>
         <v>1.3497536945812807</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="5">
+        <f t="shared" si="1"/>
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="5">
         <v>394</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="5">
         <v>1050</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="6">
         <v>1180</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="6">
         <v>2085</v>
       </c>
-      <c r="F9" s="5">
-        <f>(E9-D9)/(C9-B9)</f>
+      <c r="F9" s="7">
+        <f t="shared" si="0"/>
         <v>1.3795731707317074</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="5">
+        <f t="shared" si="1"/>
+        <v>722</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="5">
         <v>748</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="5">
         <v>1138</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="6">
         <v>1327</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="6">
         <v>1875</v>
       </c>
-      <c r="F10" s="5">
-        <f>(E10-D10)/(C10-B10)</f>
+      <c r="F10" s="7">
+        <f t="shared" si="0"/>
         <v>1.405128205128205</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="5">
+        <f t="shared" si="1"/>
+        <v>943</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="5">
         <v>603</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="5">
         <v>1069</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="6">
         <v>1389</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="6">
         <v>2050</v>
       </c>
-      <c r="F11" s="5">
-        <f>(E11-D11)/(C11-B11)</f>
+      <c r="F11" s="7">
+        <f t="shared" si="0"/>
         <v>1.4184549356223175</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="5">
+        <f t="shared" si="1"/>
+        <v>836</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="5">
         <v>732</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="5">
         <v>1104</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="6">
         <v>1296</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="6">
         <v>1844</v>
       </c>
-      <c r="F12" s="5">
-        <f>(E12-D12)/(C12-B12)</f>
+      <c r="F12" s="7">
+        <f t="shared" si="0"/>
         <v>1.4731182795698925</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="5">
+        <f t="shared" si="1"/>
+        <v>918</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="5">
         <v>736</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="5">
         <v>1085</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="6">
         <v>1320</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="6">
         <v>1850</v>
       </c>
-      <c r="F13" s="5">
-        <f>(E13-D13)/(C13-B13)</f>
+      <c r="F13" s="7">
+        <f t="shared" si="0"/>
         <v>1.518624641833811</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="5">
+        <f t="shared" si="1"/>
+        <v>910.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="5">
         <v>720</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="5">
         <v>1290</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="6">
         <v>1641</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="6">
         <v>2576</v>
       </c>
-      <c r="F14" s="5">
-        <f>(E14-D14)/(C14-B14)</f>
+      <c r="F14" s="7">
+        <f t="shared" si="0"/>
         <v>1.6403508771929824</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="5">
+        <f t="shared" si="1"/>
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="5">
         <v>683</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="5">
         <v>1068</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="6">
         <v>1399</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="6">
         <v>2046</v>
       </c>
-      <c r="F15" s="5">
-        <f>(E15-D15)/(C15-B15)</f>
+      <c r="F15" s="7">
+        <f t="shared" si="0"/>
         <v>1.6805194805194805</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="5">
+        <f t="shared" si="1"/>
+        <v>875.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="5">
         <v>595</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="5">
         <v>865</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="6">
         <v>1503</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="6">
         <v>1980</v>
       </c>
-      <c r="F16" s="5">
-        <f>(E16-D16)/(C16-B16)</f>
+      <c r="F16" s="7">
+        <f t="shared" si="0"/>
         <v>1.7666666666666666</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="5">
+        <f t="shared" si="1"/>
+        <v>730</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="5">
         <v>750</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="5">
         <v>1328</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="6">
         <v>1232</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="6">
         <v>2291</v>
       </c>
-      <c r="F17" s="5">
-        <f>(E17-D17)/(C17-B17)</f>
+      <c r="F17" s="7">
+        <f t="shared" si="0"/>
         <v>1.8321799307958477</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="5">
+        <f t="shared" si="1"/>
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="5">
         <v>600</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="5">
         <v>1107</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="6">
         <v>1473</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="6">
         <v>2411</v>
       </c>
-      <c r="F18" s="5">
-        <f>(E18-D18)/(C18-B18)</f>
+      <c r="F18" s="7">
+        <f t="shared" si="0"/>
         <v>1.8500986193293885</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="5">
+        <f t="shared" si="1"/>
+        <v>853.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="5">
         <v>766</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="5">
         <v>1066</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="6">
         <v>1497</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="6">
         <v>2065</v>
       </c>
-      <c r="F19" s="5">
-        <f>(E19-D19)/(C19-B19)</f>
+      <c r="F19" s="7">
+        <f t="shared" si="0"/>
         <v>1.8933333333333333</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="5">
+        <f t="shared" si="1"/>
+        <v>916</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="5">
         <v>850</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="5">
         <v>950</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="6">
         <v>1201</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="6">
         <v>1393</v>
       </c>
-      <c r="F20" s="5">
-        <f>(E20-D20)/(C20-B20)</f>
+      <c r="F20" s="7">
+        <f t="shared" si="0"/>
         <v>1.92</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="5">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="5">
         <v>800</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="5">
         <v>1385</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="6">
         <v>1575</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="6">
         <v>2726</v>
       </c>
-      <c r="F21" s="5">
-        <f>(E21-D21)/(C21-B21)</f>
+      <c r="F21" s="7">
+        <f t="shared" si="0"/>
         <v>1.9675213675213674</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="5">
+        <f t="shared" si="1"/>
+        <v>1092.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="5">
         <v>720</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="5">
         <v>1100</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="6">
         <v>1114</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="6">
         <v>1870</v>
       </c>
-      <c r="F22" s="5">
-        <f>(E22-D22)/(C22-B22)</f>
+      <c r="F22" s="7">
+        <f t="shared" si="0"/>
         <v>1.9894736842105263</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" s="5">
+        <f t="shared" si="1"/>
+        <v>910</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="5">
         <v>744</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="5">
         <v>1154</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="6">
         <v>1544</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="6">
         <v>2368</v>
       </c>
-      <c r="F23" s="5">
-        <f>(E23-D23)/(C23-B23)</f>
+      <c r="F23" s="7">
+        <f t="shared" si="0"/>
         <v>2.0097560975609756</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="5">
+        <f t="shared" si="1"/>
+        <v>949</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="5">
         <v>700</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="5">
         <v>1300</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="6">
         <v>1469</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="6">
         <v>2729</v>
       </c>
-      <c r="F24" s="5">
-        <f>(E24-D24)/(C24-B24)</f>
+      <c r="F24" s="7">
+        <f t="shared" si="0"/>
         <v>2.1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" s="5">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="5">
         <v>700</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="5">
         <v>900</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="6">
         <v>1509</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="6">
         <v>1933</v>
       </c>
-      <c r="F25" s="5">
-        <f>(E25-D25)/(C25-B25)</f>
+      <c r="F25" s="7">
+        <f t="shared" si="0"/>
         <v>2.12</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" s="5">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="5">
         <v>760</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="5">
         <v>1100</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="6">
         <v>1349</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="6">
         <v>2234</v>
       </c>
-      <c r="F26" s="5">
-        <f>(E26-D26)/(C26-B26)</f>
+      <c r="F26" s="7">
+        <f t="shared" si="0"/>
         <v>2.6029411764705883</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" s="5">
+        <f t="shared" si="1"/>
+        <v>930</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="5">
         <v>830</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="5">
         <v>1236</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="6">
         <v>1705</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="6">
         <v>2807</v>
       </c>
-      <c r="F27" s="5">
-        <f>(E27-D27)/(C27-B27)</f>
+      <c r="F27" s="7">
+        <f t="shared" si="0"/>
         <v>2.7142857142857144</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" s="5">
+        <f t="shared" si="1"/>
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="5">
         <v>810</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="5">
         <v>1000</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="6">
         <v>1419</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="6">
         <v>2007</v>
       </c>
-      <c r="F28" s="5">
-        <f>(E28-D28)/(C28-B28)</f>
+      <c r="F28" s="7">
+        <f t="shared" si="0"/>
         <v>3.094736842105263</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" s="5">
+        <f t="shared" si="1"/>
+        <v>905</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="5">
         <v>894</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="5">
         <v>1063</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="6">
         <v>1464</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="6">
         <v>2174</v>
       </c>
-      <c r="F29" s="5">
-        <f>(E29-D29)/(C29-B29)</f>
+      <c r="F29" s="7">
+        <f t="shared" si="0"/>
         <v>4.2011834319526624</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" s="5">
+        <f t="shared" si="1"/>
+        <v>978.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="5">
         <v>750</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="5">
         <v>975</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="6">
         <v>1099</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="6">
         <v>2299</v>
       </c>
-      <c r="F30" s="5">
-        <f>(E30-D30)/(C30-B30)</f>
+      <c r="F30" s="7">
+        <f t="shared" si="0"/>
         <v>5.333333333333333</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" s="5">
+        <f t="shared" si="1"/>
+        <v>862.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="5">
         <v>755</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="5">
         <v>855</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="6">
         <v>1301</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="6">
         <v>1908</v>
       </c>
-      <c r="F31" s="5">
-        <f>(E31-D31)/(C31-B31)</f>
+      <c r="F31" s="7">
+        <f t="shared" si="0"/>
         <v>6.07</v>
+      </c>
+      <c r="G31" s="5">
+        <f t="shared" si="1"/>
+        <v>805</v>
       </c>
     </row>
   </sheetData>
@@ -1249,5 +1384,8 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="G2:G31" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>